<commit_message>
gpt and get data
</commit_message>
<xml_diff>
--- a/starActivity.xlsx
+++ b/starActivity.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10514"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bianweizhenbian/Documents/硕士(上)/ISY5001/04 Practice Module/IDEA/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF62FDAD-C08B-2F40-9A65-6F3886A00FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D231649-EEDB-E341-8EDE-B3F350B95707}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>User ID</t>
   </si>
@@ -30,49 +30,11 @@
   <si>
     <t>Web Abstract</t>
   </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>88</t>
-  </si>
-  <si>
-    <t>53</t>
-  </si>
-  <si>
-    <t>Abstract Structural Equation/Causal Models are widely used in epidemiology and social sciences to identify and analyze the average causal effect and conditional ACE. Traditional causal effect estimation methods such as Inverse Probability Weighting and more recently Regression-With-Residuals are widely used - as they avoid the challenging task of identifying the SCM parameters - to estimate ACE and CACE. However, much work remains before traditional estimation methods can be used for counterfactual inference, and for the benefit of Personalized Public Policy Analysis in the social sciences.[BREAK]</t>
-  </si>
-  <si>
-    <t>240</t>
-  </si>
-  <si>
-    <t>Abstract Vision transformers have demonstrated impressive performance on a series of computer vision tasks, yet they still suffer from adversarial examples.[BREAK]</t>
-  </si>
-  <si>
-    <t>Compared with the pathological analysis and CT scans, the circulating tumor DNA methylation based approach is noninvasive and cost-effective, and thus is one of the most promising methods for early detection of lung cancer.[BREAK]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>404</t>
-  </si>
-  <si>
-    <t>To this end, we present SCN, a novel sparse cross-scale attention network to first align multi-scale sparse features with global voxel-encoded attention to capture the long-range relationship of instance context, which is able to boost the regression accuracy of the over-segmented large objects.[]</t>
-  </si>
-  <si>
-    <t>858</t>
-  </si>
-  <si>
-    <t>In this paper, we propose a novel multimodal conversational framework where the dialogue agent's next action and their arguments are derived jointly conditioned both on the conversational and the visual context.[]</t>
-  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -429,15 +391,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="255.83203125" collapsed="true"/>
+    <col min="3" max="3" width="255.83203125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -451,61 +413,6 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>